<commit_message>
hieu dz cty 1 10
</commit_message>
<xml_diff>
--- a/ahieu - litte - 2.xlsx
+++ b/ahieu - litte - 2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -111,15 +111,6 @@
     <t>partner</t>
   </si>
   <si>
-    <t>glass</t>
-  </si>
-  <si>
-    <t>luminous</t>
-  </si>
-  <si>
-    <t>phone Case Type</t>
-  </si>
-  <si>
     <t xml:space="preserve"> iPhone X</t>
   </si>
   <si>
@@ -147,38 +138,23 @@
     <t>dress</t>
   </si>
   <si>
-    <t>tracking Number</t>
-  </si>
-  <si>
-    <t>all1234</t>
-  </si>
-  <si>
-    <t>all1235</t>
-  </si>
-  <si>
-    <t>all1236</t>
-  </si>
-  <si>
-    <t>all1237</t>
-  </si>
-  <si>
-    <t>ck2001</t>
-  </si>
-  <si>
-    <t>ck2002</t>
-  </si>
-  <si>
-    <t>ck2003</t>
-  </si>
-  <si>
-    <t>ck2004</t>
+    <t>dr1001</t>
+  </si>
+  <si>
+    <t>dr1002</t>
+  </si>
+  <si>
+    <t>dr1003</t>
+  </si>
+  <si>
+    <t>dr1004</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,13 +291,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -668,7 +637,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -677,9 +646,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1006,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,303 +983,271 @@
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="55.42578125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="24.85546875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="28.85546875" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="55.42578125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="24.85546875" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>43750</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1">
+        <v>331038</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1">
+        <v>98515422</v>
+      </c>
+      <c r="M2" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="N2" s="1">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" s="2" t="s">
+      <c r="O2" s="2">
         <v>1</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="P2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>43751</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="2">
+        <v>10.1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>5</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>43752</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1">
+        <v>91306</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="1">
+        <v>8183262941</v>
+      </c>
+      <c r="M4" s="2">
+        <v>10.1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>5</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="Q4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>43753</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>43720</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1">
-        <v>331038</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="1">
-        <v>98515422</v>
-      </c>
-      <c r="N2" s="2">
-        <v>9.5</v>
-      </c>
-      <c r="O2" s="1">
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="1">
+        <v>91306</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="1">
+        <v>8183262941</v>
+      </c>
+      <c r="M5" s="2">
+        <v>10.1</v>
+      </c>
+      <c r="N5" s="1">
         <v>5</v>
       </c>
-      <c r="P2" s="2">
+      <c r="O5" s="2">
         <v>1</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>43721</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="2">
-        <v>10.1</v>
-      </c>
-      <c r="O3" s="1">
-        <v>5</v>
-      </c>
-      <c r="P3" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>43722</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="P5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="1">
-        <v>91306</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="1">
-        <v>8183262941</v>
-      </c>
-      <c r="N4" s="2">
-        <v>10.1</v>
-      </c>
-      <c r="O4" s="1">
-        <v>5</v>
-      </c>
-      <c r="P4" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>43722</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="1">
-        <v>91306</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="1">
-        <v>8183262941</v>
-      </c>
-      <c r="N5" s="2">
-        <v>10.1</v>
-      </c>
-      <c r="O5" s="1">
-        <v>5</v>
-      </c>
-      <c r="P5" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>